<commit_message>
fixed english translations not present in attribute fields, which are not ManyToManyFields
</commit_message>
<xml_diff>
--- a/webcentral/doc/01_data/02_tool_over/2024_05_EWB_tools_with_english_translation.xlsx
+++ b/webcentral/doc/01_data/02_tool_over/2024_05_EWB_tools_with_english_translation.xlsx
@@ -14622,7 +14622,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>WUFI (Wärme Und Feuchte Instationär) ist eine Software-Familie zur realitätsnahen instationären Berechnung Wärme- und Feuchtetransports in mehrschichtigen Bauteilen und Gebäuden unter natürlichen Klimabedingungen.</t>
+          <t>WUFI (Wärme Und Feuchte Instationär) is a software family for the realistic transient calculation of heat and moisture transport in multi-layer components and buildings under natural climatic conditions.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -14630,11 +14630,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Fraunhofer Institut für Bauphysik IBP</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -14676,7 +14672,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -14687,12 +14683,12 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Es sind mehrere Lizenzen erhältlich. Details unter https://wufi.de/de/software/lizenzen/</t>
+          <t>Several licenses are available. Details at https://wufi.de/de/software/lizenzen/</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>WUFI Plus ist das umfassendste Wärme- und Feuchtesimulationstool der WUFI-Softwarefamilie</t>
+          <t>WUFI Plus is the most comprehensive heat and humidity simulation tool in the WUFI software family</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -14707,7 +14703,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA2" t="n">
@@ -14730,7 +14726,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C# ist eine typsichere objektorientierte Allzweck-Programmiersprache.</t>
+          <t>C# is a type-safe object-oriented general-purpose programming language.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -14738,11 +14734,7 @@
           <t>Industry, Research/Teaching</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Microsoft Corporation</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -14792,7 +14784,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -14840,7 +14832,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>VSA 2.0 ist ein Werkzeug zur Erfassung und Auswertung von Daten zur Energiebilanz vieler Nichtwohngebäude. Es verfolgt als wichtiges Ziel die wissenschaftliche Analyse der Korrelation zwischen einfachen Bedarfsberechnungen mit Verbrauchsmessungen. Die Toolbox VSA 2.0 beinhaltet (1) Datenerfassungstool VSA 2.0 (gefördert von der KfW Bankengruppe), (2) TEK-Tool 9.24 mit Vorlage zur Erzeugung von Gebäude-Kurzberichten, (3) DB Tiefenerhebung (Datenmanagement für Gebäudebestände).</t>
+          <t>VSA 2.0 is a tool for collecting and analyzing data on the energy balance of many non-residential buildings. Its main objective is to scientifically analyze the correlation between simple demand calculations and consumption measurements. The VSA 2.0 toolbox includes (1) the VSA 2.0 data collection tool (sponsored by the KfW banking group), (2) TEK-Tool 9.24 with template for generating brief building reports, (3) DB Tiefenerhebung (data management for building stocks).</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -14875,7 +14867,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Die Toolchain ist in verschiedene Excel-Dateien integriert</t>
+          <t>The toolchain is integrated into various Excel files</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -14917,14 +14909,10 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Details zur Lizenz: https://github.com/IWUGERMANY/VSA-2.0---Tool-Chain/blob/main/LICENSE</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Informationen aus der Anleitung:  Systemvoraussetzungen (1) Windows Betriebssystem (Windows 7 oder neuer) (2) Installierte Microsoft Office Desktop Version (2010 oder neuer). Damit VSA 2.0 funktioniert müssen Makros in Word und Excel zugelassen werden.</t>
-        </is>
-      </c>
+          <t>License details: https://github.com/IWUGERMANY/VSA-2.0---Tool-Chain/blob/main/LICENSE</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr">
         <is>
@@ -14960,7 +14948,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BESMod ist eine quelloffene Modelica-Bibliothek, die einen modularen und benutzerfreundlichen Ansatz für bereichsübergreifende Simulationen von Energiesystemen in Gebäuden bietet und Bereiche wie Hydraulik, Lüftung, Elektrik, Steuerung und Gebäudehülle abdeckt.</t>
+          <t>BESMod is an open-source Modelica library that offers a modular and user-friendly approach for cross-domain simulations of energy systems in buildings, covering areas such as hydraulics, ventilation, electrics, controls and building envelope.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -14970,7 +14958,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
+          <t>Chair of Building and Room Air Conditioning Technology, RWTH Aachen University</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -14995,7 +14983,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>eine Modelica-Bibliothek</t>
+          <t>a Modelica library</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -15026,7 +15014,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -15041,12 +15029,12 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>Details zur Lizenz: https://github.com/RWTH-EBC/BESMod/blob/main/LICENSE</t>
+          <t>License details: https://github.com/RWTH-EBC/BESMod/blob/main/LICENSE</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>BESMOD ist eine Modulbibliothek mit standardisierten Modulen, vereinfachter abstrahierter Parametrisierung, die teilweise auf Richtlinien und Normen basiert.</t>
+          <t>BESMOD is a module library with standardized modules, simplified abstracted parameterization, which is partly based on guidelines and standards.</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -15092,7 +15080,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Die Open Energy Platform (OEP) ist ein kollaboratives, versioniertes Datensatz-Repository für die Speicherung offener Energiesystem-Modelldatensätze. Sie erleichtert die gemeinsame Nutzung, Analyse und Visualisierung von Energiedaten, um Forschung, Planung und Entscheidungsfindung im Energiesektor zu unterstützen.</t>
+          <t>The Open Energy Platform (OEP) is a collaborative, versioned dataset repository for storing open energy system model datasets. It facilitates the sharing, analysis and visualization of energy data to support research, planning and decision-making in the energy sector.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -15154,7 +15142,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -15169,7 +15157,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Der Quellcode der Open Energy Platform ist auf GitHub veröffentlicht. Das Repository ist unter der GNU Affero General Public License v3.0 (AGPL-3.0) lizenziert.</t>
+          <t>The source code of the Open Energy Platform is published on GitHub. The repository is licensed under the GNU Affero General Public License v3.0 (AGPL-3.0).</t>
         </is>
       </c>
       <c r="U6" t="inlineStr"/>
@@ -15208,7 +15196,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>React ist eine JavaScript-Bibliothek für die Entwicklung von Benutzeroberflächen. Sie ermöglicht die effiziente Erstellung von ansprechenden und interaktiven UI-Komponenten. React kann für die Entwicklung von einseitigen, mobilen oder Server-gerenderten Anwendungen verwendet werden.</t>
+          <t>React is a JavaScript library for the development of user interfaces. It enables the efficient creation of appealing and interactive UI components. React can be used for the development of single-page, mobile or server-rendered applications.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -15216,11 +15204,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Meta Open Source; React Community</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -15270,7 +15254,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -15285,7 +15269,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>MongoDB wird hauptsächlich unter einer Open-Source-Lizenz vertrieben. Es bietet jedoch auch eine kommerzielle Version mit zusätzlichen Funktionen und Support an (Details siehe https://www.mongodb.com/pricing)</t>
+          <t>MongoDB is mainly distributed under an open source license. However, it also offers a commercial version with additional functions and support (for details, see https://www.mongodb.com/pricing)</t>
         </is>
       </c>
       <c r="U7" t="inlineStr"/>
@@ -15328,7 +15312,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PostgreSQL, oft kurz Postgres genannt, ist ein freies, objektrelationales Datenbankmanagementsystem.</t>
+          <t>PostgreSQL, often called Postgres for short, is a free, object-relational database management system.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -15336,11 +15320,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>PostgreSQL Global Development Group</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization</t>
@@ -15394,7 +15374,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -15409,7 +15389,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Die PostgreSQL-License ist eine liberale Open-Source-Lizenz, die der BSD- oder MIT-Lizenz ähnlich ist.</t>
+          <t>The PostgreSQL License is a liberal open source license that is similar to the BSD or MIT license.</t>
         </is>
       </c>
       <c r="U8" t="inlineStr"/>
@@ -15452,7 +15432,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GitLab ist eine webbasierte Plattform für das DevOps-Lifecycle-Management. Sie bietet Funktionen für das Versionsmanagement von Quellcode, kontinuierliche Integration, kontinuierliche Bereitstellung, Container-Orchestrierung und mehr.</t>
+          <t>GitLab is a web-based platform for DevOps lifecycle management. It offers functions for source code version management, continuous integration, continuous deployment, container orchestration and more.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -15518,7 +15498,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -15533,7 +15513,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>GitLab wird hauptsächlich unter einer Open-Source-Lizenz vertrieben. GitLab bietet jedoch auch eine kommerzielle Version mit zusätzlichen Funktionen und Support an (Details siehe https://about.gitlab.com/pricing/).</t>
+          <t>GitLab is mainly distributed under an open source license. However, GitLab also offers a commercial version with additional functions and support (for details, see https://about.gitlab.com/pricing/).</t>
         </is>
       </c>
       <c r="U9" t="inlineStr"/>
@@ -15576,7 +15556,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SolidWorks entwickelt und vermarktet Software für computergestütztes Design, computergestütztes Engineering, 3D-CAD-Design und Zusammenarbeit, Analyse und Produktdatenmanagement. SolidWorks wird zur Erstellung von parametrischen Modellen, Baugruppen und technischen Zeichnungen verwendet.</t>
+          <t>SolidWorks develops and markets software for computer-aided design, computer-aided engineering, 3D CAD design and collaboration, analysis and product data management. SolidWorks is used to create parametric models, assemblies and technical drawings.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -15630,7 +15610,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -15641,7 +15621,7 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr">
         <is>
-          <t>Details zur Lizenzierung finden Sie hier: https://www.solidworks.com/how-to-buy/solidworks-licensing</t>
+          <t>Licensing details can be found here: https://www.solidworks.com/how-to-buy/solidworks-licensing</t>
         </is>
       </c>
       <c r="U10" t="inlineStr"/>
@@ -15680,7 +15660,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SQLite ist eine konfigurationsfreie, in sich geschlossene, eigenständige, transaktionsbezogene Datenbank-Engine, die in eine Anwendung eingebettet werden kann.</t>
+          <t>SQLite is a zero-configuration, self-contained, standalone, transactional database engine that can be embedded into an application.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -15738,7 +15718,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -15749,7 +15729,7 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
-          <t>Details zur Lizenzierung: https://www.sqlite.org/copyright.html</t>
+          <t>Licensing details: https://www.sqlite.org/copyright.html</t>
         </is>
       </c>
       <c r="U11" t="inlineStr"/>
@@ -15792,7 +15772,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OpenStudio ist eine plattformübergreifende Sammlung von Softwarewerkzeugen zur Unterstützung der Energiemodellierung ganzer Gebäude mit EnergyPlus und der erweiterten Tageslichtanalyse mit Radiance.</t>
+          <t>OpenStudio is a cross-platform collection of software tools to support whole-building energy modeling with EnergyPlus and advanced daylight analysis with Radiance.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -15800,11 +15780,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>National Renewable Energy Laboratory (USA) u. US Department of Energy; OpenStudio Coalition</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
           <t>Planning, Simulation</t>
@@ -15854,7 +15830,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -15869,7 +15845,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Details siehe https://openstudio.net/license</t>
+          <t>For details see https://openstudio.net/license</t>
         </is>
       </c>
       <c r="U12" t="inlineStr"/>
@@ -15908,7 +15884,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NANDRAD ist eine moderne Gebäudesimulationsplattform für die dynamische Bewertung der Energieeffizienz eines Gebäudes.</t>
+          <t>NANDRAD is a modern building simulation platform for the dynamic evaluation of a building's energy efficiency.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -15918,7 +15894,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Institut für Bauklimatik, TU Dresden; Bauklimatik Dresden Software GmbH</t>
+          <t>Institute for Building Climatology, TU Dresden; Bauklimatik Dresden Software GmbH</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -15943,7 +15919,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>grafische Benutzeroberfläche mit BIM HVACTool</t>
+          <t>Graphical user interface with BIM HVACTool</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -15970,7 +15946,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -15981,7 +15957,7 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
-          <t>NANDRAD als Berechnungskern kann in andere Simulationsprogramme integriert werden. Zu diesem Zweck sollte eine Lizenzierung angefragt werden.</t>
+          <t>NANDRAD as a calculation core can be integrated into other simulation programs. A license should be requested for this purpose.</t>
         </is>
       </c>
       <c r="U13" t="inlineStr"/>
@@ -15997,7 +15973,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>vor 2012</t>
+          <t>before 2012</t>
         </is>
       </c>
       <c r="AA13" t="n">
@@ -16024,7 +16000,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AixWeather ist ein Werkzeug zur Erzeugung von Wetterdaten, das für die Simulation von Energiesystemen in Gebäuden entwickelt wurde. Es wird zum Abrufen, Umwandeln und Exportieren von Wetterdaten für Forschung und Simulationen im Zusammenhang mit Gebäudeenergiesystemen verwendet.</t>
+          <t>AixWeather is a weather data generation tool designed for simulating energy systems in buildings. It is used to retrieve, transform and export weather data for research and simulations related to building energy systems.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -16034,7 +16010,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
+          <t>Chair of Building and Indoor Air Conditioning Technology, RWTH Aachen</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -16059,7 +16035,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>AixWeather Web App (https://github.com/RWTH-EBC/AixWeather-WebApp) ist eine Webanwendung zur nahtlosen Integration der Funktionen des AixWeather-Repositorys</t>
+          <t>AixWeather Web App (https://github.com/RWTH-EBC/AixWeather-WebApp) is a web application to seamlessly integrate the features of the AixWeather repository</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -16086,7 +16062,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -16101,7 +16077,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>Details zur Lizenz: https://github.com/RWTH-EBC/AixWeather/blob/main/LICENSE</t>
+          <t>License details: https://github.com/RWTH-EBC/AixWeather/blob/main/LICENSE</t>
         </is>
       </c>
       <c r="U14" t="inlineStr"/>
@@ -16144,7 +16120,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Grasshopper ist ein Plugin für Rhinoceros 3D. Es ermöglicht die Modellierung von generativen Geometrien in einem grafischen Editor. Neben einem einfachen Einstieg ist aber auch die Einbindung von Scripten und Formeln möglich.</t>
+          <t>Grasshopper is a plugin for Rhinoceros 3D. It enables the modeling of generative geometries in a graphical editor. In addition to easy access, it is also possible to integrate scripts and formulas.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -16152,11 +16128,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Robert McNeel &amp; Associates</t>
-        </is>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -16179,7 +16151,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>grafische Benutzeroberfläche (Plugin für Rhinoceros 3D)</t>
+          <t>Graphical user interface (plug-in for Rhinoceros 3D)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -16213,7 +16185,7 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
-          <t>Da Grasshopper in Rhino integriert ist: die Rhino Vollversion kann 90 Tage lang getestet werden. Nach 90 Tagen funktionieren das Speichern und die Plugins nicht mehr, es sei denn, es wird ein Lizenzschlüssel erworben. Eine Studentenversion ist ebenfalls verfügbar.</t>
+          <t>Since Grasshopper is integrated into Rhino: the Rhino full version can be tested for 90 days. After 90 days, saving and plugins will no longer work unless a license key is purchased. A student version is also available.</t>
         </is>
       </c>
       <c r="U15" t="inlineStr"/>
@@ -16256,7 +16228,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RSTAB ist ein 3D-Statik-Programm, das sich für die Berechnung von Stabwerken eignet, die in der Regel auch als Tragwerk fungieren.</t>
+          <t>RSTAB is a 3D structural analysis program that is suitable for the calculation of beam structures, which usually also function as supporting structures.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -16321,7 +16293,7 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
-          <t>Eine 90-Tage-Testversion ist verfügbar.</t>
+          <t>A 90-day trial version is available.</t>
         </is>
       </c>
       <c r="U16" t="inlineStr"/>
@@ -16360,7 +16332,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Microsoft Excel ist das am weitesten verbreitete Tabellenkalkulationsprogramm.</t>
+          <t>Microsoft Excel is the most widely used spreadsheet program.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -16368,11 +16340,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Microsoft Corporation</t>
-        </is>
-      </c>
+      <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization</t>
@@ -16418,7 +16386,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -16472,7 +16440,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>WPsource bietet ein digitales Pre-Check-Tool, welches Planern und Architekten eine Vorauswahl und Bewertung von Wärmequellen und Wärmetauschern ermöglicht.</t>
+          <t>WPsource offers a digital pre-check tool that enables planners and architects to pre-select and evaluate heat sources and heat exchangers.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -16482,7 +16450,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Steinbeis Innovationszentrum</t>
+          <t>Steinbeis Innovation Center</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -16505,11 +16473,7 @@
           <t>Miscellaneous</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Plugin für Excel</t>
-        </is>
-      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
@@ -16541,7 +16505,7 @@
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr">
         <is>
-          <t>Das Tool kann kostenfrei bezogen werden. Dazu kann eine E-Mail an franziska.bockelmann@siz-energieplus.de geschrieben werden.</t>
+          <t>The tool can be obtained free of charge. You can do this by sending an e-mail to franziska.bockelmann@siz-energieplus.de.</t>
         </is>
       </c>
       <c r="U18" t="inlineStr"/>
@@ -16557,7 +16521,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr"/>
@@ -16582,7 +16546,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Julia ist eine hochentwickelte, leistungsstarke dynamische Programmiersprache für technische Berechnungen. Sie ist für numerische und wissenschaftliche Berechnungen konzipiert.</t>
+          <t>Julia is a highly developed, powerful dynamic programming language for technical calculations. It is designed for numerical and scientific calculations.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -16640,7 +16604,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -16694,7 +16658,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>EED ist ein PC-Programm zur Auslegung vertikaler Erdwärmesonden</t>
+          <t>EED is a PC program for designing vertical borehole heat exchangers</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -16704,7 +16668,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dr. Thomas Blomberg, Blocon; Prof. Johan Claesson, Abt. für Bauphysik, Chalmers Universität, Schweden; Dr. Per Eskilson, Abt. für mathematische Physik, Universität Lund, Schweden; Prof. Göran Hellström, Abt. für mathematische Physik, Universität Lund, Schweden; Dr. Burkhard Sanner, Deutschland</t>
+          <t>Dr. Thomas Blomberg, Blocon; Prof. Johan Claesson, Dept. of Building Physics, Chalmers University, Sweden; Dr. Per Eskilson, Dept. of Mathematical Physics, Lund University, Sweden; Prof. Göran Hellström, Dept. of Mathematical Physics, Lund University, Sweden; Dr. Burkhard Sanner, germany</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -16757,11 +16721,7 @@
         </is>
       </c>
       <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>Akademische Einrichtungen erhalten 50% Rabatt.</t>
-        </is>
-      </c>
+      <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr">
@@ -16802,7 +16762,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SIM-VICUS ist eine 3D-Modellierungsumgebung für Gebäude- und Stadtteilnetze und eine innovative dynamische Simulationsmaschine.</t>
+          <t>SIM-VICUS is a 3D modeling environment for building and district networks and an innovative dynamic simulation engine.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -16812,7 +16772,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Institut für Bauklimatik, TU Dresden</t>
+          <t>Institute for Building Climatics, TU Dresden</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -16860,7 +16820,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -16914,7 +16874,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Plotly.js ist eine Bibliothek für JavaScript-Anwendungen, die Graphen und Diagramme verwenden. Es handelt sich um eine Datenvisualisierungsbibliothek, die auf D3 JS und Stack dot GL aufbaut.</t>
+          <t>Plotly.js is a library for JavaScript applications that use graphs and charts. It is a data visualization library built on top of D3 JS and Stack dot GL.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -16949,7 +16909,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>eine Javascript-Bibliothek</t>
+          <t>a Javascript library</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -16974,11 +16934,7 @@
           <t>Region/Country, Component, Facility, Building, Quarters/Networks</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>laufend</t>
-        </is>
-      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
         <is>
           <t>Open-Source, Freeware</t>
@@ -16991,7 +16947,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>Details siehe https://github.com/plotly/plotly.js?tab=License-1-ov-file</t>
+          <t>For details see https://github.com/plotly/plotly.js?tab=License-1-ov-file</t>
         </is>
       </c>
       <c r="U22" t="inlineStr"/>
@@ -17034,7 +16990,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Python ist eine universelle, üblicherweise interpretierte, höhere Programmiersprache.</t>
+          <t>Python is a universal, commonly interpreted, high-level programming language.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -17042,11 +16998,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Python Software Foundation</t>
-        </is>
-      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -17092,7 +17044,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -17107,7 +17059,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>Einige Software, die in Python integriert ist, unterliegt anderen Lizenzen.</t>
+          <t>Some software that is integrated into Python is subject to other licenses.</t>
         </is>
       </c>
       <c r="U23" t="inlineStr"/>
@@ -17154,7 +17106,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Das Modellierungsframework oemof (Open Energy Modelling Framework) ist ein Werkzeug zur Modellierung und Analyse von Energiesystemen.</t>
+          <t>The modeling framework oemof (Open Energy Modelling Framework) is a tool for modeling and analyzing energy systems.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -17270,7 +17222,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>InfluxDB ist ein Open Source Datenbankmanagementsystem, speziell für Zeitreihen.</t>
+          <t>InfluxDB is an open source database management system, especially for time series.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -17278,11 +17230,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>InfluxData Inc.</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Control, Advanced Control</t>
@@ -17336,7 +17284,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -17351,7 +17299,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>kostenlose Version verfügbar, kostenpflichtige Versionen für professionelle Anwendungen</t>
+          <t>Free version available, paid versions for professional applications</t>
         </is>
       </c>
       <c r="U25" t="inlineStr"/>
@@ -17394,7 +17342,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>pandapipes ist ein einfach zu bedienendes Netzberechnungsprogramm, das auf die Automatisierung der Analyse von Fernwärme- und Gassystemen ausgerichtet ist. Es nutzt die Datenanalysebibliothek pandas und ist auch eng mit dem Stromnetzberechnungsprogramm pandapower verwandt.</t>
+          <t>pandapipes is an easy-to-use network calculation program designed to automate the analysis of district heating and gas systems. It uses the pandas data analysis library and is also closely related to the pandapower power grid calculation program.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -17402,11 +17350,7 @@
           <t>Research/Teaching</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Das Fraunhofer-Institut für Energiewirtschaft und Energiesystemtechnik IEE; Fachgebiet Energiemanagement und Betrieb elektrischer Netze, Universität Kassel</t>
-        </is>
-      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>Simulation</t>
@@ -17429,7 +17373,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>eine Python-Bibliothek</t>
+          <t>a Python library</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -17456,7 +17400,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -17471,7 +17415,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>Details zur Lizenz: https://pandapipes.readthedocs.io/en/latest/about/license.html</t>
+          <t>License details: https://pandapipes.readthedocs.io/en/latest/about/license.html</t>
         </is>
       </c>
       <c r="U26" t="inlineStr"/>
@@ -17510,7 +17454,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SQL (steht für Structured Query Language) ist die Standardsprache für relationale Datenbankmanagementsysteme.</t>
+          <t>SQL (standing for Structured Query Language) is the standard language for relational database management systems.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -17568,7 +17512,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -17618,7 +17562,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Grafana ist eine plattformübergreifende Open-Source-Anwendung zur grafischen Darstellung von Daten aus verschiedenen Datenquellen wie z. B. InfluxDB, MySQL, PostgreSQL, Prometheus und Graphite. Die erfassten Rohdaten lassen sich anschließend in verschiedenen Anzeigeformen ausgeben.</t>
+          <t>Grafana is a cross-platform open source application for the graphical representation of data from various data sources such as InfluxDB, MySQL, PostgreSQL, Prometheus and Graphite. The captured raw data can then be output in various display formats.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -17626,11 +17570,7 @@
           <t>Service, Research/Teaching</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Grafana Labs</t>
-        </is>
-      </c>
+      <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
           <t>Monitoring, Optimization, Control</t>
@@ -17684,7 +17624,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -17699,7 +17639,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>kostenlose Version verfügbar, kostenpflichtige Versionen für professionelle Anwendungen</t>
+          <t>Free version available, paid versions for professional applications</t>
         </is>
       </c>
       <c r="U28" t="inlineStr"/>
@@ -17742,7 +17682,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>JavaScript ist eine leichtgewichtige, plattformübergreifende, interpretierte und kompilierte Programmiersprache. Sie ist auch als Skriptsprache für Webseiten bekannt, wird aber auch in vielen Nicht-Browser-Umgebungen verwendet.</t>
+          <t>JavaScript is a lightweight, cross-platform, interpreted and compiled programming language. It is also known as a scripting language for web pages, but is also used in many non-browser environments.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -17750,11 +17690,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Ecma International</t>
-        </is>
-      </c>
+      <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
           <t>Monitoring, Planning</t>
@@ -17800,7 +17736,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -17842,7 +17778,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>KNIME, der „Konstanz Information Miner“, ist eine freie Software für die interaktive Datenanalyse. KNIME ermöglicht durch das modulare Pipelining-Konzept die Integration zahlreicher Verfahren des maschinellen Lernens und des Data-Mining.</t>
+          <t>KNIME, the "Konstanz Information Miner", is free software for interactive data analysis. Thanks to its modular pipelining concept, KNIME enables the integration of numerous machine learning and data mining methods.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -17908,7 +17844,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -17923,7 +17859,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>kostenlose Version verfügbar, kostenpflichtige Versionen für professionelle Anwendungen. Für den Open-Source-Teil: Jedes Modul wird unter seiner eigenen Lizenz veröffentlicht.</t>
+          <t>free version available, paid versions for professional applications. For the open source part: Each module is published under its own license.</t>
         </is>
       </c>
       <c r="U30" t="inlineStr"/>
@@ -17966,7 +17902,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Mage ist ein Open-Source-Datenpipeline-Tool zur Transformation und Integration von Daten.</t>
+          <t>Mage is an open-source data pipeline tool for transforming and integrating data.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -18028,7 +17964,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -18086,7 +18022,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>RFEM ist eine 3D-FEM-Software zur statischen Berechnung und Bemessung von Stahl-, Stahlbeton-, Holz-, Glas- und Membran-Strukturen, für den Anlagen- und Maschinenbau sowie für dynamische Analysen.</t>
+          <t>RFEM is a 3D FEM software for the structural analysis and design of steel, reinforced concrete, timber, glass and membrane structures, for plant and mechanical engineering as well as for dynamic analyses.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -18151,7 +18087,7 @@
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
-          <t>Eine 90-Tage-Testversion ist verfügbar.</t>
+          <t>A 90-day trial version is available.</t>
         </is>
       </c>
       <c r="U32" t="inlineStr"/>
@@ -18194,7 +18130,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>GEO-HANDlight ist eine kostenlose Software, die die Planung von Erdwärmesonden unterstützt. Das Programm ermöglicht die Berechnung einzelner Erdwärmesonden bis hin zu Sondenfeldern in verschiedenen Anordnungen. Dabei werden relevante Auslegungsgrenzen überprüft, und Parameter wie Fluidtemperaturen sowie Temperaturreaktionen in der Sonde und im Erdreich können präzise bestimmt werden.</t>
+          <t>GEO-HANDlight is a free software program that supports the planning of geothermal probes. The program enables the calculation of individual geothermal probes through to probe fields in various arrangements. Relevant design limits are checked and parameters such as fluid temperatures and temperature reactions in the probe and in the ground can be precisely determined.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -18204,7 +18140,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Hochschule Biberach</t>
+          <t>Biberach University of Applied Sciences</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -18286,7 +18222,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TensorFlow ist ein Framework zur datenstromorientierten Programmierung. Populäre Anwendung findet TensorFlow im Bereich des maschinellen Lernens.</t>
+          <t>TensorFlow is a framework for data flow-oriented programming. TensorFlow is popularly used in the field of machine learning.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -18360,7 +18296,7 @@
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr">
         <is>
-          <t>Entwickelt vom Google-Brain-Team. Wird in verschiedenen Google-Produkten eingesetzt</t>
+          <t>Developed by the Google Brain team. Used in various Google products</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
@@ -18406,7 +18342,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Model Template for Residential Energy Supply Systems (MTRESS) ist ein generisches Modell für oemof.solph, das eine Vielzahl von möglichen Technologiekombinationen für Energieversorgungssysteme bietet. Es ist darauf ausgerichtet, die Energieflüsse zwischen allen Komponenten innerhalb des Systems zu berechnen und Regelungsstrategien zu optimieren, die feste Bedarfszeitreihen für Strom, Wärme und Warmwasser unter Verwendung einer beliebigen Kombination der implementierten Versorgungstechnologien erfüllen.</t>
+          <t>Model Template for Residential Energy Supply Systems (MTRESS) is a generic model for oemof.solph that provides a variety of possible technology combinations for energy supply systems. It is designed to calculate the energy flows between all components within the system and to optimize control strategies that meet fixed demand time series for electricity, heat and hot water using any combination of the implemented supply technologies.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -18416,7 +18352,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Deutsches Zentrum für Luft- und Raumfahrt e.V. (DLR); KEHAG Energiehandel GmbH</t>
+          <t>German Aerospace Center (DLR); KEHAG Energiehandel GmbH</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -18441,7 +18377,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>eine Python-Bibliothek</t>
+          <t>a Python library</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -18472,7 +18408,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -18488,7 +18424,7 @@
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr">
         <is>
-          <t>MTRESS 3.0 befindet sich in der Entwicklung und fügt die H2-Infrastruktur hinzu. Eventuell werden KPI und ein Pareto-Optimierer hinzugefügt.</t>
+          <t>MTRESS 3.0 is under development and adds the H2 infrastructure. Eventually KPI and a Pareto optimizer will be added.</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
@@ -18530,7 +18466,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SimulationX ist eine CAE-Software (Computer Aided Engineering) für die Simulation physikalisch-technischer Systeme und Anlagen.</t>
+          <t>SimulationX is a CAE software (Computer Aided Engineering) for the simulation of physical-technical systems and plants.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -18538,11 +18474,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>ESI Group</t>
-        </is>
-      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -18584,7 +18516,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -18596,7 +18528,7 @@
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr">
         <is>
-          <t>Simulationsmodelle werden auf der Basis eines diskreten Netzwerkansatzes erstellt. Das System wird in logisch zusammenhängende Teile unterteilt, welche miteinander verbunden werden.</t>
+          <t>Simulation models are created on the basis of a discrete network approach. The system is divided into logically connected parts, which are linked together.</t>
         </is>
       </c>
       <c r="V36" t="inlineStr"/>
@@ -18638,7 +18570,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Flexkälte ist eine Web-App, die entwickelt wurde, um die Flexibilität von Kälteversorgungssystemen zu erhöhen, insbesondere im Zusammenhang mit dem Ausgleich elektrischer Energie.</t>
+          <t>Flexkälte is a web app designed to increase the flexibility of refrigeration systems, especially in the context of electrical energy balancing.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -18648,7 +18580,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Umwelt-, Sicherheits- und Energietechnik UMSICHT</t>
+          <t>Fraunhofer Institute for Environmental, Safety and Energy Technology UMSICHT</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -18692,7 +18624,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -18730,7 +18662,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Simulink ist eine Software zur Modellierung von technischen, physikalischen, finanzmathematischen und anderen Systemen. Simulink ist ein Zusatzprodukt zu MATLAB und benötigt dieses zum Ausführen.</t>
+          <t>Simulink is a software for modeling technical, physical, financial mathematical and other systems. Simulink is an add-on product to MATLAB and requires MATLAB to run.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -18788,7 +18720,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -18800,7 +18732,7 @@
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr">
         <is>
-          <t>Die Modellierung erfolgt mithilfe grafischer Blöcke. Der Datefluss zwischen den Blöcken wird über gerichtete Verbindungslinien modelliert.</t>
+          <t>Modeling is carried out using graphical blocks. The data flow between the blocks is modeled using directed connecting lines.</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
@@ -18846,7 +18778,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ETA+ ist eine cloudbasierte Plattform, die Gebäudeeigentümer*innen und -manager*innen hilft, die Energieeffizienz ihrer Immobilien zu steigern. Dies wird durch die Erstellung von digitalen Abbildern (Digital Twins) jedes Gebäudes erreicht, welche alle Anlagen und Geräte umfassen. ETA+ unterstützt Nutzende dabei, Energieverbrauch zu senken und dadurch Kosten sowie klimaschädliche Emissionen zu reduzieren.</t>
+          <t>ETA+ is a cloud-based platform that helps building owners and managers increase the energy efficiency of their properties. This is achieved by creating digital images (digital twins) of each building, which include all systems and devices. ETA+ supports users in reducing energy consumption and thereby reducing costs and climate-damaging emissions.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -18900,7 +18832,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -18942,7 +18874,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>sisKMR dient zur Berechnung von Kunststoffmantelrohrleitungen und beliebigen freigelagerten, räumlichen Rohrsystemen in der Fernwärme, der Industrie und im Anlagenbau.</t>
+          <t>sisKMR is used to calculate plastic casing pipes and any freely supported, spatial pipe systems in district heating, industry and plant construction.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -19008,7 +18940,7 @@
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr">
         <is>
-          <t>Optimiert für die Berechnung von Vorwärme, Kaltverlegung, Vorspannung und erweiterte Lastfälle.</t>
+          <t>Optimized for the calculation of pre-heating, cold laying, prestressing and extended load cases.</t>
         </is>
       </c>
       <c r="V40" t="inlineStr"/>
@@ -19050,7 +18982,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>DynOpt-En ist ein dynamisches Optimierungsmodul für die angebots- und bedarfsgerechte Anbindung von Energiequellen.</t>
+          <t>DynOpt-En is a dynamic optimization module for the supply and demand-oriented connection of energy sources.</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -19058,11 +18990,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Fraunhofer-Institut für Optronik, Systemtechnik und Bildauswertung IOSB</t>
-        </is>
-      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -19104,7 +19032,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -19116,7 +19044,7 @@
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr">
         <is>
-          <t>Das Webinterface wurde in der Literatur dargestellt, aber bei unserer Aktualisierung (November 2023) sind auf der Projektwebseite weder ein Download noch weitere Informationen über das Tool verfügbar. Kommerzielle Umsetzung geplant laut Projektwebweite.</t>
+          <t>The web interface was presented in the literature, but at the time of our update (November 2023), neither a download nor further information about the tool is available on the project website. Commercial implementation planned according to the project website.</t>
         </is>
       </c>
       <c r="V41" t="inlineStr"/>
@@ -19129,7 +19057,7 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr"/>
@@ -19154,7 +19082,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ArcGIS ist der Oberbegriff für verschiedene Geoinformationssystem-Softwareprodukte des Unternehmens ESRI.</t>
+          <t>ArcGIS is the generic term for various geographic information system software products from ESRI.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -19220,7 +19148,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -19274,7 +19202,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Polysun ist eine Software, mit der sich solarthermische, photovoltaische und geothermische Anlagen effektiv simulieren lassen.</t>
+          <t>Polysun is software that can be used to effectively simulate solar thermal, photovoltaic and geothermal systems.</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -19332,7 +19260,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -19378,7 +19306,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>LS-DYNA ist ein Simulationsprogramm, das mit Hilfe der Finite-Elemente-Methode arbeitet und  auf Basis des Vorgängerprogramms DYNA3D entwickelt wurde. Insbesondere nicht-lineare und hochdynamische Problemstellungen können mit diesem Programm bearbeitet werden.</t>
+          <t>LS-DYNA is a simulation program that uses the finite element method and was developed on the basis of the predecessor program DYNA3D. In particular, non-linear and highly dynamic problems can be processed with this program.</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -19386,11 +19314,7 @@
           <t>Industry</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Livermore Software Technology Corporation (LSTC) (Ansys Inc)</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -19452,7 +19376,7 @@
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr">
         <is>
-          <t>LS-DYNA ist aus dem 1976 entwickelten 3D-FEA-Programm DYNA3D hervorgegangen.</t>
+          <t>LS-DYNA emerged from the 3D FEA program DYNA3D developed in 1976.</t>
         </is>
       </c>
       <c r="V44" t="inlineStr"/>
@@ -19490,7 +19414,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Telegraf ist ein Plugin-basierter Server Agent , welcher beim Sammeln und Versenden von Softwaremetriken unterstützt</t>
+          <t>Telegraf is a plugin-based server agent that supports the collection and sending of software metrics</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -19560,7 +19484,7 @@
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr">
         <is>
-          <t>Die Erstellung der Metriken besteht aus einem 4 stufigen Prozess. Dieser unterteilt sich in Input, Verarbeitung, Aggregation und Ausgabe.</t>
+          <t>The creation of metrics consists of a 4-stage process. This is divided into input, processing, aggregation and output.</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
@@ -19606,7 +19530,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MySQL ist ein Open-Source-Relationales Datenbanksystem, das strukturierte Daten in Tabellen speichert und durch SQL abgefragt und verwaltet wird.</t>
+          <t>MySQL is an open-source relational database management system that stores structured data in tables and is queried and managed using SQL.</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -19668,7 +19592,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -19722,7 +19646,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Simcenter STAR-CCM + ist eine kommerzielle, auf Computational Fluid Dynamics basierende Simulationssoftware</t>
+          <t>Simcenter STAR-CCM + is a commercial simulation software based on Computational Fluid Dynamics</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -19730,11 +19654,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Siemens PLM Software</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -19776,7 +19696,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -19788,7 +19708,7 @@
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr">
         <is>
-          <t>Für die Berechnung von Strömungsproblemen wird die finite Elemente- bzw. Finite Volumen methoden verwendet. Weiterhin können probleme aus dem Bereich Viskoelastizität, Turbulenz, Rheologie, Nicht- newtonische Fluide und multi-phasen Strömungen berechnet werden.</t>
+          <t>Finite element and finite volume methods are used to calculate flow problems. Furthermore, problems from the fields of viscoelasticity, turbulence, rheology, non-Newtonian fluids and multi-phase flows can be calculated.</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
@@ -19834,7 +19754,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MoniSoft ist eine plattformunabhängige Software, die das Monitoring und die Betriebsanalyse von Gebäuden vereinfacht.</t>
+          <t>MoniSoft is a platform-independent software that simplifies the monitoring and operational analysis of buildings.</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -19844,7 +19764,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Fachgebiet Bauphysik und Technischer Ausbau (fbta) am Karlsruher Institut für Technologie (KIT); Hochschule Rosenheim</t>
+          <t>Department of Building Physics and Technical Construction (fbta) at the Karlsruhe Institute of Technology (KIT); Rosenheim University of Applied Sciences</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -19919,7 +19839,7 @@
       <c r="Y48" t="inlineStr"/>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>vor 2014</t>
+          <t>before 2014</t>
         </is>
       </c>
       <c r="AA48" t="n">
@@ -19946,7 +19866,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MongoDB ist eine dokumentenorientierte NoSQL-Datenbank, die flexibles, skalierbares und leistungsstarkes Datenmanagement ermöglicht. Sie speichert Daten im BSON-Format (Binary JSON) in sogenannten Collections.</t>
+          <t>MongoDB is a document-oriented NoSQL database that enables flexible, scalable and high-performance data management. It stores data in BSON format (Binary JSON) in so-called collections.</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -19981,7 +19901,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>MongoDB Compass (grafische Benutzeroberfläche)</t>
+          <t>MongoDB Compass (graphical user interface)</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -20008,7 +19928,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -20023,7 +19943,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>MongoDB wird hauptsächlich unter einer Open-Source-Lizenz vertrieben. Es bietet jedoch auch eine kommerzielle Version mit zusätzlichen Funktionen und Support an (Details siehe https://www.mongodb.com/pricing)</t>
+          <t>MongoDB is mainly distributed under an open source license. However, it also offers a commercial version with additional functions and support (for details, see https://www.mongodb.com/pricing)</t>
         </is>
       </c>
       <c r="U49" t="inlineStr"/>
@@ -20066,7 +19986,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>OpenFOAM (Open Field Operation And Manipulation) ist eine C++-Toolbox für die Entwicklung kundenspezifischer numerischer Solver und Pre-/Post-Processing-Hilfsprogramme für die Lösung von Problemen der Kontinuumsmechanik, vor allem der numerischen Strömungsmechanik (CFD).</t>
+          <t>OpenFOAM (Open Field Operation And Manipulation) is a C++ toolbox for the development of customized numerical solvers and pre-/post-processing utilities for solving problems in continuum mechanics, especially computational fluid dynamics (CFD).</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -20101,7 +20021,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>eine C++-Toolbox</t>
+          <t>a C++ toolbox</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -20128,7 +20048,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -20186,7 +20106,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>uesgraphs ist eine Python-Bibliothek zur Beschreibung städtischer Energiesysteme und zur Verwaltung ihrer Daten in einer Python-Graphenstruktur. Die Graph-Klasse in networkx wurde erweitert, um Gebäude und Energienetze im Graphen darzustellen. uesgraphs kann als Grundlage für die Analyse von Energienetzstrukturen, die Bewertung von Fernwärmesystemen oder die Erstellung von Simulationsmodellen verwendet werden.</t>
+          <t>uesgraphs is a Python library for describing urban energy systems and managing their data in a Python graph structure. The graph class in networkx has been extended to represent buildings and energy networks in the graph. uesgraphs can be used as a basis for analyzing energy network structures, evaluating district heating systems or creating simulation models.</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -20194,11 +20114,7 @@
           <t>Service, Research/Teaching</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
-        </is>
-      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -20221,7 +20137,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>eine Python-Bibliothek</t>
+          <t>a Python library</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -20306,7 +20222,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Matlab ist eine kommerzielle Software zur Lösung mathematischer Probleme und zur grafischen Darstellung der Ergebnisse.</t>
+          <t>Matlab is a commercial software program for solving mathematical problems and displaying the results graphically.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -20364,7 +20280,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -20418,7 +20334,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Das Sustainability &amp; Impact Assessment soll insbesondere Startups dabei unterstützen ihr Geschäftsmodell auf Nachhaltigkeit anhand bestehender Normen und Methoden zu prüfen und diese für die Kommunikation an Stakeholder einheitlich aufzubereiten.</t>
+          <t>The Sustainability &amp; Impact Assessment is designed to help start-ups in particular to check their business model for sustainability using existing standards and methods and to prepare these in a standardized way for communication to stakeholders.</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -20426,11 +20342,7 @@
           <t>Industry</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Bundesverband Deutsche Startups e.V.</t>
-        </is>
-      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization</t>
@@ -20453,7 +20365,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Grafisches Tool, um die Nachhaltigkeit eines Startups zu analysieren</t>
+          <t>Graphical tool to analyze the sustainability of a startup</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
@@ -20476,7 +20388,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -20495,7 +20407,7 @@
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA53" t="n">
@@ -20522,7 +20434,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Stable Baselines3 ist eine zuverlässige, Open-Source Python-Bibliothek für Deep Reinforcement Learning (RL)-Algorithmen. Sie bietet präzise Implementierungen, die durch umfangreiche automatisierte Tests und eine einheitliche Schnittstelle unterstützt werden.</t>
+          <t>Stable Baselines3 is a reliable, open-source Python library for deep reinforcement learning (RL) algorithms. It offers precise implementations supported by extensive automated testing and a unified interface.</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -20532,7 +20444,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Institut für Robotik und Mechatronik, Deutsches Zentrum für Luft- und Raumfahrt (DLR)</t>
+          <t>Institute of Robotics and Mechatronics, German Aerospace Center (DLR)</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -20557,7 +20469,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>eine Python-Bibliothek</t>
+          <t>a Python library</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -20584,7 +20496,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -20634,7 +20546,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>TEASER (Tool for Energy Analysis and Simulation for Efficient Retrofit) ist ein offenes Werkzeug für die städtische Energiemodellierung des vorhandenen Gebäudebestands. TEASER bietet eine benutzerfreundliche Schnittstelle für verschiedene Datenquellen (z. B. CityGML, SQL, ...) sowie die Möglichkeit zur Datenanreicherung, falls erforderlich. Darüber hinaus ermöglicht TEASER den Export von gebrauchsfertigen Modelica-Simulationsmodellen für alle Bibliotheken, die die Modelica IBPSA-Bibliothek unterstützen.</t>
+          <t>TEASER (Tool for Energy Analysis and Simulation for Efficient Retrofit) is an open tool for urban energy modeling of the existing building stock. TEASER offers a user-friendly interface for different data sources (e.g. CityGML, SQL, ...) as well as the possibility for data enrichment if required. In addition, TEASER enables the export of ready-to-use Modelica simulation models for all libraries that support the Modelica IBPSA library.</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -20644,7 +20556,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
+          <t>Chair of Building and Room Air Conditioning Technology, RWTH Aachen University</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -20669,7 +20581,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>eine Python-Bibliothek</t>
+          <t>a Python Library</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -20754,7 +20666,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>IDA Indoor Climate and Energy (IDA-ICE) ist eine Software zur Simulation der Gebäudeleistung</t>
+          <t>IDA Indoor Climate and Energy (IDA-ICE) is a software for simulating building performance</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -20762,11 +20674,7 @@
           <t>Service, Research/Teaching</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>EQUA Simulation AB</t>
-        </is>
-      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -20808,7 +20716,7 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -20858,7 +20766,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Accept Mission ist eine Ideen- und Innovationsmanagement-Software zum Sammeln von Ideen, Auswählen von Ideen, Ausführen von Innovationsprojekten und Berichten über den Fortschritt. AcceptMission ist eine cloudbasierte Lösung, die den gesamten Lebenszyklus von Innovationsprojekten auf einer einheitlichen Plattform verwalten soll.</t>
+          <t>Accept Mission is an idea and innovation management software for collecting ideas, selecting ideas, executing innovation projects and reporting on progress. AcceptMission is a cloud-based solution designed to manage the entire lifecycle of innovation projects on a unified platform.</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -20893,7 +20801,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Software, cloudbasiert</t>
+          <t>Software, cloud-based</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
@@ -20912,7 +20820,7 @@
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -20931,7 +20839,7 @@
       <c r="Y57" t="inlineStr"/>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA57" t="n">
@@ -20958,7 +20866,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>EnerCalC bietet die Möglichkeit mit relativ geringem Eingabeaufwand den Energiebedarf für ein Gebäude in Anlehnung an die DIN V 18599 differenziert zu bilanzieren.</t>
+          <t>The EPN initially supports companies in positioning themselves in a digital ecosystem. In addition, the tool offers assistance in identifying suitable business model patterns that can ultimately be combined to form a specific business model.</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -20968,7 +20876,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Institut für Gebäude-Energieforschung, Dr. Markus Lichtmeß</t>
+          <t>Institute for Building Energy Research, Dr. Markus Lichtmeß</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -20993,7 +20901,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>grafische Benutzeroberfläche (Plugin für Excel)</t>
+          <t>Graphical user interface (plug-in for Excel)</t>
         </is>
       </c>
       <c r="K58" t="inlineStr"/>
@@ -21016,7 +20924,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -21062,7 +20970,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>T*SOL ist ein dynamisches Simulationsprogramm zur Auslegung, Optimierung und Berechnung von solarthermischen Anlagen.</t>
+          <t>T*SOL is a dynamic simulation program for the design, optimization and calculation of solar thermal systems.</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -21070,11 +20978,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Valentin Software GmbH</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -21116,7 +21020,7 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -21127,7 +21031,7 @@
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr">
         <is>
-          <t>Eine 30-Tage-Testversion ist verfügbar.</t>
+          <t>A 30-day trial version is available.</t>
         </is>
       </c>
       <c r="U59" t="inlineStr"/>
@@ -21170,7 +21074,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Highcharts ist eine JavaScript-Diagrammbibliothek, die es ermöglicht, interaktive und visuell ansprechende Diagramme für Webanwendungen zu erstellen.</t>
+          <t>Highcharts is a JavaScript chart library that makes it possible to create interactive and visually appealing charts for web applications.</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -21178,11 +21082,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Highsoft</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
           <t>Monitoring</t>
@@ -21228,7 +21128,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -21243,7 +21143,7 @@
       </c>
       <c r="T60" t="inlineStr">
         <is>
-          <t>Die Quellcodes sind auf der Produktwebsite verfügbar. Das Herunterladen und Ausprobieren von Produkten ist kostenlos. Sobald ein Projekt/Produkt für die Markteinführung bereit ist, ist der Erwerb einer kommerziellen Lizenz erforderlich. Es ist auch möglich, eine Bildungslizenz zu erwerben, die eine kostenlose Nutzung für nicht-kommerzielle Projekte für ein Jahr ermöglicht.</t>
+          <t>The source codes are available on the product website. Downloading and testing products is free of charge. As soon as a project/product is ready for market launch, the purchase of a commercial license is required. It is also possible to purchase an educational license, which allows free use for non-commercial projects for one year.</t>
         </is>
       </c>
       <c r="U60" t="inlineStr"/>
@@ -21290,7 +21190,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>HOWAmonitor ist ein eingebettetes System, das die Effektivität und Effizienz von RLT-Anlagen überwacht und die sämtliche Anlagenzustände speichert und bewertet.</t>
+          <t>HOWAmonitor is an embedded system that monitors the effectiveness and efficiency of HVAC systems and records and evaluates all system states.</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -21344,7 +21244,7 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -21367,7 +21267,7 @@
       <c r="Y61" t="inlineStr"/>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA61" t="n">
@@ -21394,7 +21294,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Mit dem Simulationsprogramm DIBS (Dynamic ISO Building Simulator) lässt sich der Endenergiebedarf für Heizung und Kühlung von Nichtwohngebäuden (NWG) in Deutschland mit geringem Aufwand berechnen.</t>
+          <t>The DIBS (Dynamic ISO Building Simulator) simulation program can be used to calculate the final energy demand for heating and cooling of non-residential buildings in Germany with little effort.</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -21404,7 +21304,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Institut Wohnen und Umwelt GmbH</t>
+          <t>Institute for Housing and the Environment</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -21452,7 +21352,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -21506,7 +21406,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Methodenentwicklung zur Erstellung von Simulationsmodellen aus Daten des Building Information Modeling.</t>
+          <t>Method development for the creation of simulation models from Building Information Modeling data.</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -21516,7 +21416,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen; Lehrstuhl für Energieeffizientes Bauen, RWTH Aachen; ROM Technik GmbH</t>
+          <t>Chair of Building and Air Conditioning Technology, RWTH Aachen University; Chair of Energy Efficient Building, RWTH Aachen University; ROM Technik GmbH</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -21568,7 +21468,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -21622,7 +21522,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Erstellung einer digitalen Funktionsbeschreibung der Steuer- und Regelungsfunktionen individueller Gebäude.</t>
+          <t>Creation of a digital functional description of the control and regulation functions of individual buildings.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -21676,7 +21576,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -21722,7 +21622,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">VBA (Visual Basic for Applications) ist eine von Microsoft entwickelte Programmiersprache, die hauptsächlich für die Automatisierung von Aufgaben in Office-Anwendungen verwendet wird. Mit VBA können Benutzer Makros schreiben, um wiederholende Aufgaben automatisch auszuführen, wie das Zusammenstellen von Daten, das Erstellen von Berichten und das Anpassen von Funktionen. </t>
+          <t>VBA (Visual Basic for Applications) is a programming language developed by Microsoft, primarily used for automating tasks in Office applications. With VBA, users can write macros to automatically perform repetitive tasks, such as compiling data, creating reports, and customizing functions.</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -21780,7 +21680,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -21830,7 +21730,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Naotilus ist eine innovative, modular erweiterbare Überwachungsplattform für das kollaborative technische Management von Fernwärmesystemen. Naotilus ermöglicht die gleichzeitige Digitalisierung der Instandhaltung und die kontinuierliche Überwachung der technischen Anlagen.</t>
+          <t>Naotilus is an innovative, modularly expandable monitoring platform for the collaborative technical management of district heating systems. Naotilus enables the simultaneous digitalization of maintenance and continuous monitoring of technical systems.</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -21884,7 +21784,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -21930,7 +21830,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>FEFLOW (Finite Element subsurface FLOW System) ist ein Computerprogramm zur Simulation des Grundwasserflusses, des Stoffübergangs und des Wärmeübergangs in porösen und gebrochenen Medien.</t>
+          <t>FEFLOW (Finite Element subsurface FLOW System) is a computer program for the simulation of groundwater flow, mass transfer and heat transfer in porous and fractured media.</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -21938,11 +21838,7 @@
           <t>Service, Research/Teaching</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>DHI</t>
-        </is>
-      </c>
+      <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation</t>
@@ -21984,7 +21880,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -21995,7 +21891,7 @@
       <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr">
         <is>
-          <t>Es sind verschiedene Lizenzen erhältlich, darunter auch eine akademische Lizenz für Studierende und Forschungseinrichtungen.</t>
+          <t>Various licenses are available, including an academic license for students and research institutions.</t>
         </is>
       </c>
       <c r="U67" t="inlineStr"/>
@@ -22042,7 +21938,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>GHEtool ist ein Werkzeug für Bohrfeldberechnungen. GHEtools bietet Zugang zu der Technologie, die notwendig ist, um die geothermische Entwicklung zu beschleunigen und die Machbarkeit geothermischer Lösungen zu erleichtern.</t>
+          <t>GHEtool is a tool for drilling field calculations. GHEtools provides access to the technology necessary to accelerate geothermal development and facilitate the feasibility of geothermal solutions.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -22100,7 +21996,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -22115,7 +22011,7 @@
       </c>
       <c r="T68" t="inlineStr">
         <is>
-          <t>Eine Pro-Version ist verfügbar und die Preise sind unter https://ghetool.eu/pricing/ aufgeführt.</t>
+          <t>A Pro version is available and prices are listed at https://ghetool.eu/pricing/.</t>
         </is>
       </c>
       <c r="U68" t="inlineStr"/>
@@ -22150,7 +22046,7 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CAD (computer-aided-design) bezeichnet die Unterstützung von konstruktiven Aufgaben mittels EDV zur Herstellung eines Produkts.</t>
+          <t>CAD (computer-aided design) refers to the support of design tasks using EDP to manufacture a product.</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -22208,7 +22104,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -22250,7 +22146,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Rhinoceros 3D ist eine Software für die computergestützte 3D-Modellierung und das rechnergestützte Konstruieren.</t>
+          <t>Rhinoceros 3D is a software for computer-aided 3D modeling and computer-aided design.</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -22258,11 +22154,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Robert McNeel &amp; Associates</t>
-        </is>
-      </c>
+      <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -22323,7 +22215,7 @@
       <c r="S70" t="inlineStr"/>
       <c r="T70" t="inlineStr">
         <is>
-          <t>Die Vollversion kann 90 Tage lang getestet werden. Nach 90 Tagen funktionieren das Speichern und die Plugins nicht mehr, es sei denn, es wird ein Lizenzschlüssel erworben. Eine Studentenversion ist ebenfalls verfügbar.</t>
+          <t>Rhinoceros 3D is a software for computer-aided 3D modeling and computer-aided design, the full version can be tested for 90 days. After 90 days, saving and plug-ins will no longer work unless a license key is purchased. A student version is also available.</t>
         </is>
       </c>
       <c r="U70" t="inlineStr"/>
@@ -22366,7 +22258,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>TimescaleDB ist eine Open-Source-SQL-Datenbank für Zeitreihen, die PostgresSQL erweitert und für schnelle Sammlungen und komplexe Abfragen optimiert ist.</t>
+          <t>TimescaleDB is an open source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries.</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -22374,11 +22266,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Timescale Inc.</t>
-        </is>
-      </c>
+      <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
           <t>Monitoring</t>
@@ -22428,7 +22316,7 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -22443,7 +22331,7 @@
       </c>
       <c r="T71" t="inlineStr">
         <is>
-          <t>Details siehe https://github.com/timescale/timescaledb/blob/main/LICENSE</t>
+          <t>TimescaleDB is an open source SQL database for time series that extends PostgresSQL and is optimized for fast collections and complex queries.for details see https://github.com/timescale/timescaledb/blob/main/LICENSE</t>
         </is>
       </c>
       <c r="U71" t="inlineStr"/>
@@ -22486,7 +22374,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>OpenModelica ist eine kostenlose Open Source-Umgebung, die auf der Modelica-Modellierungssprache zum Modellieren, Simulieren, Optimieren und Analysieren komplexer dynamischer Systeme basiert.</t>
+          <t>OpenModelica is a free open source environment based on the Modelica modeling language for modeling, simulating, optimizing and analyzing complex dynamic systems.</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -22494,11 +22382,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Open Source Modelica Consortium (OSMC)</t>
-        </is>
-      </c>
+      <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization, Simulation</t>
@@ -22548,7 +22432,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -22602,7 +22486,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Microsoft Visio ist ein Visualisierungsprogramm von Microsoft für Windows.</t>
+          <t>Microsoft Visio is a visualization program from Microsoft for Windows.</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -22660,7 +22544,7 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -22710,7 +22594,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>R ist eine freie Softwareumgebung für statistische Berechnungen und Grafiken.</t>
+          <t>R is a free software environment for statistical calculations and graphics.</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -22772,7 +22656,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -22830,7 +22714,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Das BIEC-Phasenmodell hilft in fünf Schritten bei der Entwicklung von Geschäftsmodellinnovationen. Dabei werden für jeden Schritt Tools und Methoden angeboten, die online und offline beim Prozess unterstützen können.</t>
+          <t>The BIEC phase model helps with the development of business model innovations in five steps. Tools and methods are offered for each step that can support the process both online and offline.</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -22840,7 +22724,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Arbeitswirtschaft und Organisation IAO</t>
+          <t>Fraunhofer Institute for Industrial Engineering IAO</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -22880,7 +22764,7 @@
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -22899,7 +22783,7 @@
       <c r="Y75" t="inlineStr"/>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA75" t="n">
@@ -22926,7 +22810,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ITONICS Innovation OS soll jede Phase des Innovationprozesses managen. Die Innovationsmanagement-Software kann individuell für Teams und Unternehmen angepasst werden, in bestehende Prozesse integriert werden und die Innovation unternehmensweit verankern.</t>
+          <t>ITONICS Innovation OS is designed to manage every phase of the innovation process. The innovation management software can be customized for teams and companies, integrated into existing processes and anchor innovation throughout the company.</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -22976,7 +22860,7 @@
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -23022,7 +22906,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>IfcOpenShell ist eine Open-Source-Softwarebibliothek, die in C++ und Python verfügbar ist und die Arbeit mit dem Industry Foundation Classes (IFC)-Dateiformat erleichtern soll. Das IFC-Dateiformat kann zur Beschreibung von Gebäude- und Konstruktionsdaten verwendet werden und wird üblicherweise für Building Information Modelling eingesetzt.</t>
+          <t>IfcOpenShell is an open source software library, available in C++ and Python, designed to facilitate work with the Industry Foundation Classes (IFC) file format. The IFC file format can be used to describe building and construction data and is commonly used for Building Information Modeling.</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -23084,7 +22968,7 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -23134,7 +23018,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>DELPHIN ist eine Simulationssoftware für gekoppelten Wärme-, Feuchte-, Luft- und Salztransport in porösen Baustoffen.</t>
+          <t>DELPHIN is a simulation software for coupled heat, moisture, air and salt transport in porous building materials.</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -23144,7 +23028,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Institut für Bauklimatik, TU Dresden</t>
+          <t>Institute for Building Climatics, TU Dresden</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -23192,7 +23076,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -23250,7 +23134,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MasterSim ist ein Co-Simulations-Masterprogramm, welches die Mock-Up-Interface (FMI)-Co-Simulation unterstützt. MasterSim verbindet verschiedene Simulationsmodelle und tauscht Daten zwischen Simulation-Slaves zur Laufzeit aus.</t>
+          <t>MasterSim is a co-simulation master program that supports mock-up interface (FMI) co-simulation. MasterSim connects different simulation models and exchanges data between simulation slaves at runtime.</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -23258,11 +23142,7 @@
           <t>Research/Teaching, Service, Industry</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Dr. Andreas Nicolai von Bauklimatik Dresden Software GmbH</t>
-        </is>
-      </c>
+      <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -23312,7 +23192,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -23366,7 +23246,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Das Functional Mock-up Interface (FMI) ist ein freier Standard, der den Austausch dynamischer Modelle mithilfe einer Kombination aus XML-Dateien, Binärdateien und C-Code, die in einer einzigen Datei gezippt sind, ermöglicht.</t>
+          <t>The Functional Mock-up Interface (FMI) is a free standard that enables the exchange of dynamic models using a combination of XML files, binary files and C code zipped into a single file.</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -23374,11 +23254,7 @@
           <t>Industry, Research/Teaching</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Modelica Association</t>
-        </is>
-      </c>
+      <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation, Control, Advanced Control</t>
@@ -23478,7 +23354,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Der EPN unterstützt Unternehmen zunächst bei der Positionierung in einem digitalen Ökosystem. Darüber hinaus bietet das Tool Hilfestellungen zur Identifikation von passenden Geschäftsmodellmustern, die schließlich zu einem spezifischen Geschäftsmodell kombiniert werden können.</t>
+          <t>The EPN initially supports companies in positioning themselves in a digital ecosystem. In addition, the tool offers assistance in identifying suitable business model patterns that can ultimately be combined to form a specific business model.</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -23486,11 +23362,7 @@
           <t>Industry</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Fraunhofer-Institut für Arbeitswirtschaft und Organisation IAO</t>
-        </is>
-      </c>
+      <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
           <t>Planning</t>
@@ -23528,7 +23400,7 @@
       <c r="P81" t="inlineStr"/>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -23547,7 +23419,7 @@
       <c r="Y81" t="inlineStr"/>
       <c r="Z81" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA81" t="n">
@@ -23574,7 +23446,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SIR 3S ist ein Softwaretool, das für die Berechnung, Simulation, Analyse und Optimierung von Strömungsvorgängen in Gas-, Wasser- und Wärmeversorgungsnetzen sowie anderen Rohrleitungssystemen entwickelt wurde.</t>
+          <t>SIR 3S is a software tool developed for the calculation, simulation, analysis and optimization of flow processes in gas, water and heat supply networks as well as other piping systems.</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -23628,7 +23500,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -23674,7 +23546,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ENTIGRIS ist ein Strommarktmodell zur Analyse von Energiesystemen aus einer ökonomischen Perspektive. Es berücksichtigt verschiedene Faktoren, darunter Akteurskonstellationen und wirtschaftliche Indikatoren, um Einblicke in die Entwicklung von Energiesystemen zu geben.</t>
+          <t>ENTIGRIS is an electricity market model for analyzing energy systems from an economic perspective. It takes into account various factors, including actor constellations and economic indicators, to provide insights into the development of energy systems.</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -23728,7 +23600,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -23772,7 +23644,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Eclipse Mosquitto ist ein open source (EPL/EDL licensed) message broker, welcher mit dem MQTT protocol arbeitet</t>
+          <t>Eclipse Mosquitto is an open source (EPL/EDL licensed) message broker that works with the MQTT protocol</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -23830,7 +23702,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -23884,7 +23756,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>AutoCAD ist eine CAD-Software, die Architekten, Ingenieure und Baufachleute zur Erstellung präziser 2D- und 3D-Zeichnungen einsetzen.</t>
+          <t>AutoCAD is CAD software used by architects, engineers and construction specialists to create precise 2D and 3D drawings.</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -23950,7 +23822,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -23996,7 +23868,7 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Gombis 2.0 ermöglicht eine wirtschaftliche Optimierung von Energieeinsparmaßnahmen an Gebäuden (Geb.-Hülle, Lüftung) und eine Simulation von Energiesystemen (Kessel, BHKW, Wärmepumpen; PV) zur Nutzwärme-Bereitstellung und Eigenstromerzeugung für einzelne Gebäude oder für Quartiere mit der Möglichkeit einer iterativen Optimierung. Es dient als Werkzeug zur energetischen Optimierung von Quartieren in der Phase der Konzeptentwicklung. Gombis 20 basiert auf zwei Vorläufer- Modellen (1) zur Optimierung von gebäudeseitigen Energiesparmaßnahmen („V-ROM“) und (2) zur Simulation von BHKW-Systemen („Gombis 1.0“), die in einem Modell integriert wurden, wobei die Simulation des Energiesystems auf den gebäudeseitig optimierten Gebäuden beruht.</t>
+          <t>Gombis 2.0 enables economic optimization of energy saving measures in buildings (building envelope, ventilation) and simulation of energy systems (boilers, cogeneration plants, heat pumps; PV) for the provision of useful heat and self-generated electricity for individual buildings or for districts with the possibility of iterative optimization . It serves as a tool for the energy optimization of neighborhoods in the concept development phase. Gombis 20 is based on two previous models (1) for optimizing building energy saving measures (“V-ROM”) and (2) for simulating CHP systems (“Gombis 1.0”), which were integrated into one model, with the simulation of the energy system is based on the buildings being optimized.</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -24006,7 +23878,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>G. Korb / Dr. Jank Energieplanung</t>
+          <t>G. Korb / Dr. Jank energy planning</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -24106,7 +23978,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Der KI-Navigator zeigt anhand von Beispielen, welche Aufgaben die Künstliche Intelligenz in der Dienstleistungsentwicklung und im Dienstleistungsmanagement übernehmen kann. Für jede Phase des Dienstleistungslebenszyklus sind typische Aktivitäten aufgelistet, zu denen – sofern vorhanden – am Markt verfügbare KI-Lösungen und Praxisbeispiele hinterlegt sind.</t>
+          <t>The AI Navigator uses examples to show which tasks artificial intelligence can take on in service development and service management. Typical activities are listed for each phase of the service life cycle, for which AI solutions available on the market and practical examples are provided where available.</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -24116,7 +23988,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Arbeitswirtschaft und Organisation IAO</t>
+          <t>Fraunhofer Institute for Industrial Engineering IAO</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -24156,7 +24028,7 @@
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -24175,7 +24047,7 @@
       <c r="Y87" t="inlineStr"/>
       <c r="Z87" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA87" t="inlineStr"/>
@@ -24200,7 +24072,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Framework zum Erstellen neuralen Netze zur Objekterkennung</t>
+          <t>Framework for creating neural networks for object recognition</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -24262,7 +24134,7 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -24316,7 +24188,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Windheizung 2.0 Planungstool ist eine Software zur Planung und Optimierung von Windheizung 2.0 Gebäuden, die überschüssige Windenergie zum Heizen nutzen.</t>
+          <t>Wind Heating 2.0 Planning Tool is a software for planning and optimizing Wind Heating 2.0 buildings that use surplus wind energy for heating.</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -24326,7 +24198,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Bauphysik IBP</t>
+          <t>Fraunhofer Institute for Building Physics IBP</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -24416,7 +24288,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Bei der mondas® IoT-Plattform handelt es sich um ein webbasiertes Analysetool, das speziell für große Datenmengen ausgelegt ist. Die Plattform kann vielfältige Aufgaben wie Energie- und Anlagenmonitoring, Inbetriebnahme-Monitoring, Predictive Maintenance oder Logistik übernehmen. Für die Überwachung eignen sich Anlagen wie Blockheizkraftwerke, Solaranlagen, aber auch Kältemaschinen, Druckluftkompressoren sowie die gesamte Gebäudetechnik in großen Liegenschaften und komplexen Verwaltungsgebäuden.</t>
+          <t>The mondas® IoT platform is a web-based analysis tool that is specially designed for large volumes of data. The platform can take on a wide range of tasks such as energy and system monitoring, commissioning monitoring, predictive maintenance and logistics. Systems such as combined heat and power plants, solar systems, but also chillers, air compressors and the entire building technology in large properties and complex administrative buildings are suitable for monitoring.</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -24424,11 +24296,7 @@
           <t>Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>mondas GmbH</t>
-        </is>
-      </c>
+      <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization</t>
@@ -24470,7 +24338,7 @@
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
@@ -24493,7 +24361,7 @@
       <c r="Y90" t="inlineStr"/>
       <c r="Z90" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA90" t="n">
@@ -24520,7 +24388,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Der Quartiersgenerator ist ein Webtool zum Vergleich von Versorgungskonzepten für Quartiere. Es enthält einen Lastprofilgenerator für indivisualisiebaren Gebäudebstand in Quartier, eine Auslegungsoptimierung zentraler Versorgungsysteme, Betriebsoptimierung verschiedener Technologieszenarien und Bewertung anhand KPIs.</t>
+          <t>The district generator is a web tool for comparing supply concepts for districts. It contains a load profile generator for customizable building stock in districts, design optimization of central supply systems, operational optimization of various technology scenarios and evaluation based on KPIs.</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -24530,7 +24398,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
+          <t>Chair of Building and Room Air Conditioning Technology, RWTH Aachen University</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -24582,7 +24450,7 @@
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R91" t="inlineStr">
@@ -24609,7 +24477,7 @@
       <c r="Y91" t="inlineStr"/>
       <c r="Z91" t="inlineStr">
         <is>
-          <t>2022 /2024 (geplannt als ein Webtool)</t>
+          <t>2022 /2024 (planned as a web tool)</t>
         </is>
       </c>
       <c r="AA91" t="n">
@@ -24632,7 +24500,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>DolphinDB ist eine hochleistungsfähige Zeitreihendatenbank. Sie ist mit einer benutzerfreundlichen, voll funktionsfähigen Programmiersprache und einem hochvolumigen, schnellen Streaming-Analysesystem integriert.</t>
+          <t>DolphinDB is a high-performance time series database. It is integrated with an easy-to-use, full-featured programming language and a high-volume, fast streaming analysis system.</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -24640,11 +24508,7 @@
           <t>Research/Teaching, Service, Administration, Industry</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>DolphinDB, Inc.</t>
-        </is>
-      </c>
+      <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
           <t>Miscellaneous</t>
@@ -24690,7 +24554,7 @@
       </c>
       <c r="Q92" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R92" t="inlineStr">
@@ -24744,7 +24608,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>aedifion ist eine cloudbasierte Plattform zur Überwachung, Optimierung und Steuerung von Gebäuden. Sie vereint Gebäudeautomation, Heizungs-, Lüftungs- und Klimaanlagen (HLK), Energiesysteme, Aufzüge, Zutrittskontrollsysteme, Beleuchtung und vieles mehr in einem strukturierten Datenpool für einen effektiven energie- und kosteneffizienten Anlagenbetrieb.</t>
+          <t>aedifion is a cloud-based platform for monitoring, optimizing and controlling buildings. It combines building automation, heating, ventilation and air conditioning (HVAC), energy systems, elevators, access control systems, lighting and much more in a structured data pool for effective energy and cost-efficient system operation.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -24798,7 +24662,7 @@
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R93" t="inlineStr">
@@ -24848,7 +24712,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Modelica ist eine objektorientierte Modellierungssprache für physikalische Modelle.</t>
+          <t>Modelica is an object-oriented modeling language for physical models.</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -24906,7 +24770,7 @@
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R94" t="inlineStr">
@@ -24960,7 +24824,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Dymola ist eine kommerzielle Modellierungs- und Simulationsumgebung basierend auf der offenen Modellierungssprache Modelica.</t>
+          <t>Dymola is a commercial modeling and simulation environment based on the open modeling language Modelica.</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -25068,7 +24932,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Das Cockpit soll eine erste Orientierungshilfe zum Thema Digitalisierung im Unternehmen anbieten. Es besteht aus einer beständig wachsenden Sammlung von Unternehmensbeispielen aus unterschiedlichen Branchen mit konkreten Anhaltspunkten und Denkanstößen für eine Digitalisierungsstrategie.</t>
+          <t>The Cockpit is intended to provide initial guidance on the topic of digitalization in companies. It consists of a constantly growing collection of company examples from various sectors with concrete points of reference and food for thought for a digitalization strategy.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -25078,7 +24942,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>RKW Rationalisierungs- und Innovationszentrum der Deutschen Wirtschaft e. V.</t>
+          <t>RKW Rationalization and Innovation Center of German Business e. V.</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -25122,7 +24986,7 @@
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R96" t="inlineStr">
@@ -25168,7 +25032,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>EnergyConnect ist ein modernes Echtzeit-Leitsystem, das verschiedene dezentrale Energieanlagen zusammenfasst, steuert und überwacht. Es kann als das virtuelle Kraftwerk beschrieben werden.</t>
+          <t>EnergyConnect is a modern real-time control system that combines, controls and monitors various decentralized energy systems. It can be described as the virtual power plant.</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -25178,7 +25042,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Energiewirtschaft und Energiesystemtechnik IEE</t>
+          <t>Fraunhofer Institute for Energy Economics and Energy System Technology IEE</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -25226,7 +25090,7 @@
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R97" t="inlineStr">
@@ -25272,7 +25136,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>CloneMAP (cloud-native Multi-Agent Plattform) ist eine Multi-Agenten Plattform, welche für die Ausführung in einem Kubernetes-Cluster entwickelt wurde. Das Ziel dieses Projekts ist es, die Vorteile von Cloud-Computing und einem verteilten Programmierparadigma (Multi-Agenten Systeme) zu kombinieren. cloneMAP ist in der Programmiersprache Go geschrieben.</t>
+          <t>CloneMAP (cloud-native multi-agent platform) is a multi-agent platform designed to run in a Kubernetes cluster. The goal of this project is to combine the advantages of cloud computing and a distributed programming paradigm (multi-agent systems). cloneMAP is written in the Go programming language.</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -25384,7 +25248,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t xml:space="preserve">HovalSupervisor ist ein Online-Leitsystem zur Visualisierung und Betreuung von Energieanlagen und -systemen via Browser für gewerbliche Anwendungen (u. a. Wohnbau, Hotellerie), sowie Fernwärmenetze. Verschiedene Informationen wie Fehlermeldungen können visualisiert werden. </t>
+          <t>HovalSupervisor is an online control system for the visualization and management of energy systems and installations via a browser for commercial applications (e.g., residential buildings, hotels), as well as district heating networks. Various information such as error messages can be visualized.</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -25438,7 +25302,7 @@
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R99" t="inlineStr">
@@ -25461,7 +25325,7 @@
       <c r="Y99" t="inlineStr"/>
       <c r="Z99" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA99" t="n">
@@ -25488,7 +25352,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>EHDO (Energy hub design optimization) ist ein Webtool zur Unterstützung des Planungsprozesses von komplexen Energieversorgungssystemen. EHDO unterstützt die Planung zukünftiger Energieversorgungssysteme und die Abschätzung des Potenzials von erneuerbaren Energien und zukünftigen Energieträgern wie Wasserstoff. Eine breite Palette innovativer Technologien wie Brennstoffzellen, Elektrolyseure, Wasserstoffspeicher, Photovoltaik- und Windkraftanlagen sowie Biomasse- und Waste-to-Energy-Technologien können in dem Tool berücksichtigt werden.</t>
+          <t>EHDO (Energy hub design optimization) is a web tool to support the planning process of complex energy supply systems. EHDO supports the planning of future energy supply systems and the assessment of the potential of renewable energies and future energy sources such as hydrogen. A wide range of innovative technologies such as fuel cells, electrolyzers, hydrogen storage, photovoltaic and wind power plants as well as biomass and waste-to-energy technologies can be taken into account in the tool.</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -25498,7 +25362,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Lehrstuhl für Gebäude- und Raumklimatechnik, RWTH Aachen</t>
+          <t>Chair of Building and Room Air Conditioning Technology, RWTH Aachen University</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -25596,7 +25460,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>COMSOL Multiphysics ist eine Software zur Simulation physikalischer Vorgänge, die mittels Differentialgleichungen beschrieben werden können.</t>
+          <t>COMSOL Multiphysics is a software for the simulation of physical processes that can be described by means of differential equations.</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -25700,7 +25564,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>GenSim ist ein Werkzeug zur Simulation der Strom- und Wärmebedarfs von Gebäuden, mit einem Fokus auf den frühen Entwurfsphasen. Es kann hochauflösende zeitliche Daten verarbeiten und vereinfacht geometrische Modelle für effiziente Simulationen.</t>
+          <t>GenSim is a tool for simulating the electricity and heat demand of buildings, with a focus on the early design phases. It can process high-resolution temporal data and simplifies geometric models for efficient simulations.</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -25758,7 +25622,7 @@
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R102" t="inlineStr">
@@ -25816,7 +25680,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Der SWIVT-Controller ist ein umfassendes Werkzeug, das in den SWIVT-Projekten zur Optimierung der Auslegung und des Betriebs des Energiesystems des SWIFT-Quartiers eingesetzt wird.</t>
+          <t>The SWIVT Controller is a comprehensive tool used in the SWIVT projects to optimize the design and operation of the SWIFT district energy system.</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -25824,11 +25688,7 @@
           <t>Research/Teaching, Service</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Institut für Mechatronische Systeme im Maschinenbau, Technische Universität Darmstadt</t>
-        </is>
-      </c>
+      <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
           <t>Monitoring, Planning, Optimization</t>
@@ -25870,7 +25730,7 @@
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R103" t="inlineStr">
@@ -25912,7 +25772,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Der Business Model Canvas (BMC) dient zur Visualisierung von Geschäftsmodellen und soll dabei helfen, innovative Geschäftsmodelle zu entwickeln oder bestehende Geschäftsmodelle zu verändern. Im Mittelpunkt steht dabei die Geschäftslogik eines Unternehmens oder Angebots.</t>
+          <t>The Business Model Canvas (BMC) is used to visualize business models and is intended to help develop innovative business models or change existing business models. The focus is on the business logic of a company or offering.</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -25958,7 +25818,7 @@
       <c r="P104" t="inlineStr"/>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R104" t="inlineStr">
@@ -26004,7 +25864,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>DesignBuilder für Ingenieure dient u.a. zur Unterstützung bei der nachhaltigen Gebäudeplanung. Führende Dienstleistungsingenieure und Energiemodellierer verwenden DesignBuilder, um Designentscheidungen zu treffen, die Energieeffizienz, Komfort und Kosten optimieren.</t>
+          <t>DesignBuilder for Engineers is used, among other things, to support sustainable building design. Leading service engineers and energy modelers use DesignBuilder to make design decisions that optimize energy efficiency, comfort and cost.</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -26108,7 +25968,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>EnergyPlus ist ein Gebäudeenergie-Simulationsprogramm für Ingenieure und Architekten um sowohl den Energieverbrauch für Heizung, Kühlung, Lüftung, Beleuchtung sowie Plug-and-Process-Lasten und den Wasserverbrauch in Gebäuden zu modellieren und zu simulieren.</t>
+          <t>EnergyPlus is a building energy simulation program for engineers and architects to model and simulate energy consumption for heating, cooling, ventilation, lighting as well as plug-and-process loads and water consumption in buildings.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -26118,7 +25978,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>EnergyPlus wird vom Building Technologies Office (BTO) des US-Energieministeriums (DOE) gefördert und vom National Renewable Energy Laboratory (NREL) betreut.</t>
+          <t>EnergyPlus is sponsored by the Building Technologies Office (BTO) of the U.S. Department of Energy (DOE) and managed by the National Renewable Energy Laboratory (NREL).</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -26166,7 +26026,7 @@
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R106" t="inlineStr">
@@ -26220,7 +26080,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>nPro ist eine Software für die frühe Planungsphase von Quartieren und Wärmenetzen. Es umfasst die technische Auslegung von Quartierslösungen (Wärmenetze, LowEx-Netze, kalte Nahwärme) und die Berechnung der Wirtschaftlichkeit.</t>
+          <t>nPro is a software tool for the early planning phase of districts and heat networks. It includes the technical design of district energy solutions (conventional heat networks, lowex networks, 5GDHC networks) and the calculation of their profitability.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -26282,7 +26142,7 @@
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R107" t="inlineStr">
@@ -26328,7 +26188,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>CasADi ist ein Open-Source-Softwaretool für numerische Optimierung im Allgemeinen und optimale Steuerung (d.h. Optimierung mit Differentialgleichungen) im Besonderen.</t>
+          <t>CasADi is an open source software tool for numerical optimization in general and optimal control (i.e. optimization with differential equations) in particular.</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -26386,7 +26246,7 @@
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R108" t="inlineStr">
@@ -26436,7 +26296,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>TAS ist eine hochspezialisierte Software für die thermische Optimierung von Gebäuden, die es ermöglicht, Einflüsse von Luftbewegungen, Sonnenstrahlung sowie Erwärmungs- und Kühlprozesse an Gebäuden zu simulieren.</t>
+          <t>TAS is a highly specialized software for the thermal optimization of buildings, which makes it possible to simulate the influences of air movements, solar radiation and heating and cooling processes on buildings.</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -26444,11 +26304,7 @@
           <t>Research/Teaching, Service</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>Environmental Design Solutions Ltd</t>
-        </is>
-      </c>
+      <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr">
         <is>
           <t>Visualization, Planning, Optimization, Simulation</t>
@@ -26536,7 +26392,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>IdeaCheck soll einen professionellen, wissenschaftlich validierten Fragebogen aus der Produktidee heraus generieren. Es wird eine demographisch passende Zielgruppe für die Idee befragt. IdeaCheck erstellt ein ausgewogenes, unvoreingenommenes Ergebnis, sowie eine Bewertung der Idee, inklusive Kommentaren von Umfrageteilnehmenden.</t>
+          <t>IdeaCheck is designed to generate a professional, scientifically validated questionnaire from the product idea. A demographically suitable target group for the idea is surveyed. IdeaCheck produces a balanced, unbiased result, as well as an evaluation of the idea, including comments from survey participants.</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -26586,7 +26442,7 @@
       <c r="P110" t="inlineStr"/>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R110" t="inlineStr">
@@ -26632,7 +26488,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>X3DOM ist ein quelloffenes JavaScript-Framework zur Erstellung deklarativer 3D-Szenen in Webseiten. Kurz gesagt bedeutet das deklarative 3D-Konzept, dass man eine interaktive 3D-Szene mit Hilfe einer strukturierten, textuellen Darstellung erstellen und anzeigen kann, anstatt Code zu schreiben - und zwar ohne ein Plugin in den Browsern. Im Fall von X3DOM ist diese textuelle Darstellung Teil eines HTML-Dokuments, das eine Webseite darstellt. Auf diese Weise wird der 3D-Inhalt zu einem Bürger erster Klasse innerhalb der Webseite, genau wie Text, Links, Bilder oder Filme.</t>
+          <t>X3DOM is an open-source JavaScript framework for creating declarative 3D scenes in websites. In short, the declarative 3D concept means that you can create and display an interactive 3D scene using a structured, textual representation instead of writing code - without a plugin in the browsers. In the case of X3DOM, this textual representation is part of an HTML document that represents a web page. In this way, the 3D content becomes a first-class citizen within the web page, just like text, links, images or movies.</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -26642,7 +26498,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Graphische Datenverarbeitung IGD</t>
+          <t>Fraunhofer Institute for Computer Graphics Research IGD</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -26690,7 +26546,7 @@
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R111" t="inlineStr">
@@ -26740,7 +26596,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Django ist ein in Python geschriebenes, quelloffenes Webframework,  das schnelle Entwicklung und ein sauberes, pragmatisches Design fördert.</t>
+          <t>Django is an open-source web framework written in Python that promotes rapid development and clean, pragmatic design.</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -26806,7 +26662,7 @@
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R112" t="inlineStr">
@@ -26864,7 +26720,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Das BIEC-Canvas unterstützt anhand von Leitfragen die Ausarbeitung eines Business Modell Canvas speziell für digitale Geschäftsmodelle. Die Unterlagen können als PDF runtergeladen oder sofort online genutzt werden.</t>
+          <t>The BIEC Canvas uses guiding questions to support the development of a business model canvas specifically for digital business models. The documents can be downloaded as a PDF or used immediately online.</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -26874,7 +26730,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Arbeitswirtschaft und Organisation IAO</t>
+          <t>Fraunhofer Institute for Industrial Engineering IAO</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -26914,7 +26770,7 @@
       <c r="P113" t="inlineStr"/>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R113" t="inlineStr">
@@ -26933,7 +26789,7 @@
       <c r="Y113" t="inlineStr"/>
       <c r="Z113" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA113" t="n">
@@ -26960,7 +26816,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>QGIS ist eine freie Geoinformationssystemsoftware zum Betrachten, Bearbeiten, Erfassen und Analysieren räumlicher Daten.</t>
+          <t>QGIS is a free geographic information system software for viewing, editing, capturing and analyzing spatial data.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -27026,7 +26882,7 @@
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R114" t="inlineStr">
@@ -27084,7 +26940,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>OpenGeoSys (OGS) ist ein wissenschaftliches Open-Source-Projekt zur Entwicklung numerischer Methoden zur Simulation von thermo-hydro-mechanisch-chemischen (THMC) Prozessen in porösen und gebrochenen Medien.</t>
+          <t>OpenGeoSys (OGS) is a scientific open source project for the development of numerical methods for the simulation of thermo-hydro-mechanical-chemical (THMC) processes in porous and fractured media.</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -27094,7 +26950,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Helmholtz-Zentrum für Umweltforschung GmbH (UFZ); the OpenGeoSys community</t>
+          <t>Helmholtz Center for Environmental Research GmbH (UFZ); the OpenGeoSys community</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -27146,7 +27002,7 @@
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R115" t="inlineStr">
@@ -27200,7 +27056,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>CO2Calc4Quartier ist ein Tool, das für die Bewertung von Fernwärmekonzepten mit besonderem Fokus auf CO2-Emissionen entwickelt wurde.</t>
+          <t>CO2Calc4Quartier is a tool that was developed for evaluating district heating concepts with a particular focus on CO2 emissions.</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -27210,7 +27066,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Fachgebiet Energiewirtschaft, Brandenburgische Technische Universität Cottbus-Senftenberg; r2b energy consulting GmbH; BTB Blockheizkraftwerks-, Träger- und Betreibergesellschaft mbH Berlin</t>
+          <t>Department of Energy Economics, Brandenburg Technical University Cottbus-Senftenberg; r2b energy consulting GmbH; BTB Combined heat and power plant, carrier and operator company mbH Berlin</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -27250,7 +27106,7 @@
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R116" t="inlineStr">
@@ -27271,7 +27127,7 @@
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>voraussichtlich 2024</t>
+          <t>expected in 2024</t>
         </is>
       </c>
       <c r="AA116" t="inlineStr"/>
@@ -27292,7 +27148,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>MonKey ist  eine Analyse- und Visualisierungsplattform, die die Datenflut aus Monitoring (Mon) und Anlagenkennschlüssel (Key) mit ausgefeilten Big-Data-Methoden in leicht verständliche Informationen umwandelt.</t>
+          <t>MonKey is an analysis and visualization platform that converts the flood of data from monitoring (Mon) and system keys (Key) into easily understandable information using sophisticated big data methods.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -27302,7 +27158,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>EGS-plan Ingenieurgesellschaft für Energie-, Gebäude- und Solartechnik mbH</t>
+          <t>EGS-plan engineering company for energy, building and solar technology mbH</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -27346,7 +27202,7 @@
       </c>
       <c r="Q117" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R117" t="inlineStr">
@@ -27365,7 +27221,7 @@
       <c r="Y117" t="inlineStr"/>
       <c r="Z117" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="AA117" t="n">
@@ -27392,7 +27248,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Die Toolbox "Geschäftsmodellentwicklung im Mittelstand" enthält eine Sammlung von Tools, die einen Geschäftsmodellentwicklungsprozess bereichern können. Zu jedem Tool gibt es eine Anleitung in PDF Format sowie eine Wordvorlage zum Anpassen und Ausdrucken.</t>
+          <t>The toolbox "Business model development in SMEs" contains a collection of tools that can enrich a business model development process. Each tool comes with instructions in PDF format and a Word template for customizing and printing.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -27402,7 +27258,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>RKW Rationalisierungs- und Innovationszentrum der Deutschen Wirtschaft e. V.</t>
+          <t>RKW Rationalization and Innovation Center of German Business e. V.</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -27446,7 +27302,7 @@
       </c>
       <c r="Q118" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R118" t="inlineStr">
@@ -27492,7 +27348,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Mit der ANSYS Fluids Produktfamilie für Strömungsmechanik steht Ingenieuren ein breites Portfolio technisch führender Technologien für das gesamte Anwendungsspektrum der Fluidsimulation zur Verfügung, mit denen sie den Einfluss von Fluidströmungen auch bei komplexen Wechselwirkungen zwischen verschiedenen physikalischen Einflussfaktoren sowie beweglichen Geometrien zuverlässig ermitteln können.</t>
+          <t>The ANSYS Fluids product family for fluid mechanics provides engineers with a broad portfolio of technically leading technologies for the entire application spectrum of fluid simulation, with which they can reliably determine the influence of fluid flows, even with complex interactions between different physical influencing factors and moving geometries.</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -27550,7 +27406,7 @@
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R119" t="inlineStr">
@@ -27604,7 +27460,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>MetricX ist eine software, die weder von der Plattform noch vom System abhängt und dazu dient, umfangreiche technische Betriebsdaten aus Fernwärmesystemen mit hoher zeitlicher Genauigkeit zu erfassen, zu verarbeiten und zu analysieren.</t>
+          <t>MetricX is software that does not depend on the platform or the system and is used to collect, process and analyze extensive technical operational data from district heating systems with high temporal accuracy.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -27614,7 +27470,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Institut für nachhaltige Energieversorgung GmbH; Technische Hochschule Rosenheim</t>
+          <t>Institute for Sustainable Energy Supply GmbH; Rosenheim Technical University</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -27658,7 +27514,7 @@
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R120" t="inlineStr">
@@ -27700,7 +27556,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>TRNSYS (abgekürzt: TRaNsient SYstems Simulation) ist eine flexible, grafisch basierte, modulare Softwareumgebung, die es ermöglicht, das Verhalten transienter Systeme zu simulieren, daher der Name.</t>
+          <t>TRNSYS (abbreviation: TRaNsient SYstems Simulation) is a flexible, graphically based, modular software environment that makes it possible to simulate the behavior of transient systems, hence the name.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -27754,7 +27610,7 @@
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R121" t="inlineStr">
@@ -27765,7 +27621,7 @@
       <c r="S121" t="inlineStr"/>
       <c r="T121" t="inlineStr">
         <is>
-          <t>Kostenpflichtig, günstiger für Hochschulen, Source-Code wird nach Erwerb zur Verfügung gestellt. Eine kostenlose Testversion mit begrenztem Funktionsumfang kann auf der Herstellerseite heruntergeladen werden.</t>
+          <t>Chargeable, cheaper for universities, source code is made available after purchase. A free trial version with limited functionality can be downloaded from the manufacturer's website.</t>
         </is>
       </c>
       <c r="U121" t="inlineStr"/>
@@ -27804,7 +27660,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Das Simulationsprogramm THERAKLES berechnet das dynamische thermische oder hygrothermische Verhalten von Räumen und Gebäuden. Es ist ein Berechnungswerkzeug für planende Ingenieure und Architekten im Bereich der Bauphysik, des Bauklimas und der technischen Gebäudeausrüstung.</t>
+          <t>The THERAKLES simulation program calculates the dynamic thermal or hygrothermal behavior of rooms and buildings. It is a calculation tool for planning engineers and architects in the field of building physics, building climate and technical building equipment.</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -27812,11 +27668,7 @@
           <t>Service, Research/Teaching</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>Dr. Andreas Nicolai, Dr.-Ing. Peggy Freudenberg und Dipl.-Ing. Heiko Fechner von Bauklimatik Dresden Software GmbH</t>
-        </is>
-      </c>
+      <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr">
         <is>
           <t>Planning, Optimization, Simulation</t>
@@ -27858,7 +27710,7 @@
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R122" t="inlineStr">
@@ -27869,7 +27721,7 @@
       <c r="S122" t="inlineStr"/>
       <c r="T122" t="inlineStr">
         <is>
-          <t>THERAKLES ist als kostenfreie und kommerzielle Professional-Version verfügbar. Die freie Version ist hinsichtlich der Verwendung in kommerziellen Projekten nicht eingeschränkt. Details siehe https://www.bauklimatik-dresden.de/therakles/bestellen.php?aLa=de</t>
+          <t>THERAKLES is available as a free and commercial professional version. The free version is not restricted for use in commercial projects. For details see https://www.bauklimatik-dresden.de/therakles/bestellen.php?aLa=de</t>
         </is>
       </c>
       <c r="U122" t="inlineStr"/>
@@ -27908,7 +27760,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Resie (Rechenkern für die Simulation von Energiesystemen) ist ein Simulationswerkzeug zur Simulation und Optimierung verschiedener Energieversorgungssysteme für Stadtteile oder Einzelgebäude mit dem Fokus auf Betriebsstrategien, das bereits in frühen Planungsphasen eingesetzt werden kann.</t>
+          <t>Resie (calculation kernel for the simulation of energy systems) is a simulation tool for simulating and optimizing various energy supply systems for urban districts or individual buildings with a focus on operating strategies, which can already be used in the early planning phases.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -27966,7 +27818,7 @@
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>laufend</t>
+          <t>ongoing</t>
         </is>
       </c>
       <c r="R123" t="inlineStr">
@@ -28016,7 +27868,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>PostProc 2 ist eine Software für die Analyse und Nachbearbeitung von zeitabhängigen Daten, die z.B. in dynamischen Simulationsprogrammen oder aus Messdaten erzeugt werden.</t>
+          <t>PostProc 2 is a software for the analysis and post-processing of time-dependent data generated, for example, in dynamic simulation programs or from measurement data.</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -28026,7 +27878,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Dr. Andreas Nicolai und Dipl.-Ing. Heiko Fechner von Bauklimatik Dresden Software GmbH</t>
+          <t>Dr. Andreas Nicolai and Dipl.-Ing. Heiko Fechner from Bauklimatik Dresden Software GmbH</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -28112,7 +27964,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>EQ-City ist ein Planungswerkzeug bzw. eine Software, die sich auf Energieversorgungskonzepte in Quartieren und Städten bezieht. Es kann genutzt werden, um transparente Investitionsentscheidungen zur Wärmeversorgung in städtischen Gebieten zu treffen.</t>
+          <t>EQ-City is a planning tool or software that relates to energy supply concepts in neighborhoods and cities. It can be used to make transparent investment decisions for heat supply in urban areas.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -28122,7 +27974,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Energiewirtschaft und Energiesystemtechnik IEE</t>
+          <t>Fraunhofer Institute for Energy Economics and Energy System Technology IEE</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -28162,7 +28014,7 @@
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R125" t="inlineStr">
@@ -28202,7 +28054,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>investSCOPE optimiert Transformationspfade für die Dekarbonisierung von Erzeugungsportfolios unter Berücksichtigung finanzieller Kennziffern und bestimmt, in welche Technologie zu welchem Zeitpunkt und zu welchen Kosten investiert werden sollte, um einen wirtschaftlich optimalen Pfad zur Portfolioentwicklung zu erreichen.</t>
+          <t>investSCOPE optimizes transformation paths for the decarbonization of generation portfolios, taking financial metrics into account and determines which technology should be invested in, at what time and at what cost, in order to achieve an economically optimal path for portfolio development.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -28212,7 +28064,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Fraunhofer-Institut für Energiewirtschaft und Energiesystemtechnik IEE</t>
+          <t>Fraunhofer Institute for Energy Economics and Energy System Technology IEE</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -28260,7 +28112,7 @@
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R126" t="inlineStr">
@@ -28294,7 +28146,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>E2M2 (European Electricity Market Model) ist ein grundlegendes Strommarktmodell, das mit dem Ziel entwickelt wurde, die Systemkosten auf dem europäischen Strommarkt zu minimieren.</t>
+          <t>E2M2 (European Electricity Market Model) is a basic electricity market model developed with the aim of minimizing system costs in the European electricity market.</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -28304,7 +28156,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Institut für Energiewirtschaft und rationelle Energieanwendung (IER), Universität Stuttgart</t>
+          <t>Institute for Energy Economics and Rational Energy Use (IER), University of Stuttgart</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -28344,7 +28196,7 @@
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R127" t="inlineStr">
@@ -28378,7 +28230,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>EnergyMap Berlin ist eine Online-Plattform zur Erstellung eines gebäudespezifischen digitalen Wärmekatasters für den Gebäudebestand des Landes Berlin. Das gebäudescharfe Wärmekataster ist ein Werkzeug der kommunalen Wärmeplanung. Es erfasst alle beheizten Gebäude in den einzelnen Kommunen des Landkreises und beinhaltet zu jedem Gebäude Informationen zu Nutzung, Baustruktur und Wärmebedarf.</t>
+          <t>EnergyMap Berlin is an online platform for creating a building-specific digital heat register for the building stock of the state of Berlin. The building-specific heat register is a tool for municipal heat planning. It records all heated buildings in the individual municipalities of the district and contains information on usage, building structure and heat requirements for each building.</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -28388,7 +28240,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>co2online gemeinnützige Beratungsgesellschaft mbH</t>
+          <t>co2online non-profit consulting company mbH</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -28432,7 +28284,7 @@
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>unbekannt</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R128" t="inlineStr">

</xml_diff>